<commit_message>
Removed old files; Upgraded synch
</commit_message>
<xml_diff>
--- a/data/db.xlsx
+++ b/data/db.xlsx
@@ -375,9 +375,6 @@
     <t>2013-03-30 08:15:00</t>
   </si>
   <si>
-    <t>asset</t>
-  </si>
-  <si>
     <t>app_audit_log</t>
   </si>
   <si>
@@ -415,6 +412,9 @@
   </si>
   <si>
     <t>cell</t>
+  </si>
+  <si>
+    <t>customer</t>
   </si>
 </sst>
 </file>
@@ -779,7 +779,7 @@
   <dimension ref="A1:T85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +859,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -874,10 +874,10 @@
         <v>1</v>
       </c>
       <c r="K3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -933,10 +933,10 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
@@ -961,7 +961,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -1580,10 +1580,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B43" t="s">
         <v>120</v>
-      </c>
-      <c r="B43" t="s">
-        <v>121</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C44" t="s">
         <v>23</v>
@@ -1614,7 +1614,7 @@
         <v>33</v>
       </c>
       <c r="E45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C46" t="s">
         <v>11</v>
@@ -1636,7 +1636,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C47" t="s">
         <v>23</v>
@@ -1650,7 +1650,7 @@
         <v>110</v>
       </c>
       <c r="C48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F48">
         <v>0</v>

</xml_diff>